<commit_message>
Add project documentation, updated charts and png versions of them
</commit_message>
<xml_diff>
--- a/Software Project 1/Source/results/cnn_fashionmnist.xlsx
+++ b/Software Project 1/Source/results/cnn_fashionmnist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stefan\GitHub\MachineLearning\Software Project 1\Source\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DC7A68A-C3C3-450A-A87E-8E02E8670B60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB46C32-93D3-4475-B2EE-A4F403DE706D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2894,12 +2894,12 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
               <a:t>CNN (FashionMNIST)</a:t>
             </a:r>
-            <a:endParaRPr lang="ro-RO">
+            <a:endParaRPr lang="ro-RO" sz="1100">
               <a:effectLst/>
             </a:endParaRPr>
           </a:p>
@@ -2908,12 +2908,12 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
               <a:t>Test Loss</a:t>
             </a:r>
-            <a:endParaRPr lang="ro-RO">
+            <a:endParaRPr lang="ro-RO" sz="1100">
               <a:effectLst/>
             </a:endParaRPr>
           </a:p>
@@ -5930,16 +5930,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>293370</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>7620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>998220</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1223010</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>7620</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5966,16 +5966,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>716280</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1379220</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6038,16 +6038,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>632460</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>71</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>30480</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6075,13 +6075,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1043940</xdr:colOff>
+      <xdr:colOff>640080</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>7620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1089660</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1066800</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>7620</xdr:rowOff>
     </xdr:to>
@@ -6410,8 +6410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>